<commit_message>
Cleaned up 3D model, and added part list and costing overview
</commit_message>
<xml_diff>
--- a/part list.xlsx
+++ b/part list.xlsx
@@ -9,6 +9,7 @@
   </bookViews>
   <sheets>
     <sheet name="Part list" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Main procurements" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -19,8 +20,50 @@
 </workbook>
 </file>
 
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <authors>
+    <author> </author>
+  </authors>
+  <commentList>
+    <comment ref="A2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Jean-Marc Wislez:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">- oven + stenen
+- ovensturing
+- 2 hoofdsteunen
+- zandloper
+- thermo/hygrometer
+- verlichting
+- verluchting</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="107">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -260,16 +303,98 @@
   </si>
   <si>
     <t xml:space="preserve">Door (TBW)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Top bench (TBW)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lower bench (TBW)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Heater protection (TBW)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Electricity (TBW)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sauna-heater + accessories</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2ehands.be</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wood (structure)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gijsbrechts n.v.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OSB-plates</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Woodtex</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sauna wood (second choice)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">saunahaus.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Base beams terrace</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Slating battens</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gamma</t>
+  </si>
+  <si>
+    <t xml:space="preserve">External wood (second choice)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bofa nv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2x 12m glasswool 60cm/10cm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Iso-Technics</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4x 8m glasswool 60cm/15cm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thermally hardened glas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dirk Walschaerts bvba</t>
+  </si>
+  <si>
+    <t xml:space="preserve">energie-shop.net</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Electricity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NV J. Piscaer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Small items and consumables</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TOTAL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="#,##0.00\ [$€-80C];[RED]\-#,##0.00\ [$€-80C]"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="11">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -295,6 +420,49 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <i val="true"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -345,7 +513,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -358,7 +526,43 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -379,10 +583,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E74"/>
+  <dimension ref="A1:E82"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A43" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A74" activeCellId="0" sqref="A74"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -411,13 +615,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-    </row>
+    <row r="2" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
         <v>5</v>
@@ -444,7 +642,7 @@
       <c r="A5" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C5" s="0" t="n">
@@ -453,7 +651,7 @@
       <c r="D5" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="4" t="s">
         <v>9</v>
       </c>
     </row>
@@ -470,7 +668,7 @@
       <c r="D6" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" s="4" t="s">
         <v>9</v>
       </c>
     </row>
@@ -512,7 +710,7 @@
       <c r="A9" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="4" t="s">
         <v>22</v>
       </c>
       <c r="C9" s="0" t="n">
@@ -521,7 +719,7 @@
       <c r="D9" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="E9" s="4" t="s">
         <v>21</v>
       </c>
     </row>
@@ -538,7 +736,7 @@
       <c r="D10" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="E10" s="4" t="s">
         <v>9</v>
       </c>
     </row>
@@ -546,8 +744,11 @@
       <c r="A11" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="4" t="s">
         <v>15</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>1</v>
       </c>
       <c r="D11" s="0" t="s">
         <v>27</v>
@@ -579,7 +780,7 @@
       <c r="A15" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="4" t="s">
         <v>32</v>
       </c>
       <c r="C15" s="0" t="n">
@@ -588,58 +789,58 @@
       <c r="D15" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="E15" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="16" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="3" t="s">
+      <c r="E15" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C16" s="3" t="n">
+      <c r="C16" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="D16" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="E16" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="17" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="3" t="s">
+      <c r="E16" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C17" s="3" t="n">
+      <c r="C17" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="D17" s="3" t="s">
+      <c r="D17" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="E17" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="18" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="3" t="s">
+      <c r="E17" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="C18" s="3" t="n">
+      <c r="C18" s="4" t="n">
         <v>22</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="D18" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="E18" s="3" t="s">
+      <c r="E18" s="4" t="s">
         <v>40</v>
       </c>
     </row>
@@ -664,7 +865,7 @@
       <c r="A20" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B20" s="4" t="s">
         <v>43</v>
       </c>
       <c r="C20" s="0" t="n">
@@ -673,24 +874,24 @@
       <c r="D20" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="E20" s="3" t="s">
+      <c r="E20" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="21" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="3" t="s">
+    <row r="21" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B21" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C21" s="3" t="n">
+      <c r="C21" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="D21" s="3" t="s">
+      <c r="D21" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="E21" s="3" t="s">
+      <c r="E21" s="4" t="s">
         <v>47</v>
       </c>
     </row>
@@ -728,20 +929,20 @@
         <v>53</v>
       </c>
     </row>
-    <row r="24" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="3" t="s">
+    <row r="24" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="B24" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C24" s="3" t="n">
+      <c r="C24" s="4" t="n">
         <v>13</v>
       </c>
-      <c r="D24" s="3" t="s">
+      <c r="D24" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="E24" s="3" t="s">
+      <c r="E24" s="4" t="s">
         <v>56</v>
       </c>
     </row>
@@ -771,7 +972,7 @@
       <c r="A28" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="B28" s="3" t="s">
+      <c r="B28" s="4" t="s">
         <v>32</v>
       </c>
       <c r="C28" s="0" t="n">
@@ -780,126 +981,126 @@
       <c r="D28" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="E28" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="29" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="3" t="s">
+      <c r="E28" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="29" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B29" s="3" t="s">
+      <c r="B29" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C29" s="3" t="n">
+      <c r="C29" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="D29" s="3" t="s">
+      <c r="D29" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="E29" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="30" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="3" t="s">
+      <c r="E29" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="30" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B30" s="3" t="s">
+      <c r="B30" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="C30" s="3" t="n">
+      <c r="C30" s="4" t="n">
         <v>22</v>
       </c>
-      <c r="D30" s="3" t="s">
+      <c r="D30" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="E30" s="3" t="s">
+      <c r="E30" s="4" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="31" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="3" t="s">
+    <row r="31" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B31" s="3" t="s">
+      <c r="B31" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C31" s="3" t="n">
+      <c r="C31" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="D31" s="3" t="s">
+      <c r="D31" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E31" s="3" t="s">
+      <c r="E31" s="4" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="32" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="3" t="s">
+    <row r="32" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B32" s="3" t="s">
+      <c r="B32" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="C32" s="3" t="n">
+      <c r="C32" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="D32" s="3" t="s">
+      <c r="D32" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="E32" s="3" t="s">
+      <c r="E32" s="4" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="33" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="3" t="s">
+    <row r="33" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B33" s="3" t="s">
+      <c r="B33" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="C33" s="3" t="n">
+      <c r="C33" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="D33" s="3" t="s">
+      <c r="D33" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E33" s="3" t="s">
+      <c r="E33" s="4" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="34" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="3" t="s">
+    <row r="34" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B34" s="3" t="s">
+      <c r="B34" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="C34" s="3" t="n">
+      <c r="C34" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="D34" s="3" t="s">
+      <c r="D34" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="E34" s="3" t="s">
+      <c r="E34" s="4" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="35" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="3" t="s">
+    <row r="35" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B35" s="3" t="s">
+      <c r="B35" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="C35" s="3" t="n">
+      <c r="C35" s="4" t="n">
         <v>13</v>
       </c>
-      <c r="D35" s="3" t="s">
+      <c r="D35" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="E35" s="3" t="s">
+      <c r="E35" s="4" t="s">
         <v>56</v>
       </c>
     </row>
@@ -929,7 +1130,7 @@
       <c r="A39" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="B39" s="3" t="s">
+      <c r="B39" s="4" t="s">
         <v>32</v>
       </c>
       <c r="C39" s="0" t="n">
@@ -938,126 +1139,126 @@
       <c r="D39" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="E39" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="40" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="3" t="s">
+      <c r="E39" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="40" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B40" s="3" t="s">
+      <c r="B40" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C40" s="3" t="n">
+      <c r="C40" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="D40" s="3" t="s">
+      <c r="D40" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="E40" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="41" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="3" t="s">
+      <c r="E40" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="41" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B41" s="3" t="s">
+      <c r="B41" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="C41" s="3" t="n">
+      <c r="C41" s="4" t="n">
         <v>22</v>
       </c>
-      <c r="D41" s="3" t="s">
+      <c r="D41" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="E41" s="3" t="s">
+      <c r="E41" s="4" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="42" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="3" t="s">
+    <row r="42" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B42" s="3" t="s">
+      <c r="B42" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C42" s="3" t="n">
+      <c r="C42" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="D42" s="3" t="s">
+      <c r="D42" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E42" s="3" t="s">
+      <c r="E42" s="4" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="43" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="3" t="s">
+    <row r="43" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B43" s="3" t="s">
+      <c r="B43" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="C43" s="3" t="n">
+      <c r="C43" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="D43" s="3" t="s">
+      <c r="D43" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="E43" s="3" t="s">
+      <c r="E43" s="4" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="44" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="3" t="s">
+    <row r="44" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B44" s="3" t="s">
+      <c r="B44" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="C44" s="3" t="n">
+      <c r="C44" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="D44" s="3" t="s">
+      <c r="D44" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E44" s="3" t="s">
+      <c r="E44" s="4" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="45" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="3" t="s">
+    <row r="45" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B45" s="3" t="s">
+      <c r="B45" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="C45" s="3" t="n">
+      <c r="C45" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="D45" s="3" t="s">
+      <c r="D45" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="E45" s="3" t="s">
+      <c r="E45" s="4" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="46" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="3" t="s">
+    <row r="46" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B46" s="3" t="s">
+      <c r="B46" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="C46" s="3" t="n">
+      <c r="C46" s="4" t="n">
         <v>13</v>
       </c>
-      <c r="D46" s="3" t="s">
+      <c r="D46" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="E46" s="3" t="s">
+      <c r="E46" s="4" t="s">
         <v>56</v>
       </c>
     </row>
@@ -1087,7 +1288,7 @@
       <c r="A50" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="B50" s="3" t="s">
+      <c r="B50" s="4" t="s">
         <v>32</v>
       </c>
       <c r="C50" s="0" t="n">
@@ -1096,58 +1297,58 @@
       <c r="D50" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="E50" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="51" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="3" t="s">
+      <c r="E50" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="51" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B51" s="3" t="s">
+      <c r="B51" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C51" s="3" t="n">
+      <c r="C51" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="D51" s="3" t="s">
+      <c r="D51" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="E51" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="52" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="3" t="s">
+      <c r="E51" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="52" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B52" s="3" t="s">
+      <c r="B52" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C52" s="3" t="n">
+      <c r="C52" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="D52" s="3" t="s">
+      <c r="D52" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="E52" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="53" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="3" t="s">
+      <c r="E52" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="53" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B53" s="3" t="s">
+      <c r="B53" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C53" s="3" t="n">
+      <c r="C53" s="4" t="n">
         <v>44</v>
       </c>
-      <c r="D53" s="3" t="s">
+      <c r="D53" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="E53" s="3" t="s">
+      <c r="E53" s="4" t="s">
         <v>70</v>
       </c>
     </row>
@@ -1172,7 +1373,7 @@
       <c r="A55" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="B55" s="3" t="s">
+      <c r="B55" s="4" t="s">
         <v>71</v>
       </c>
       <c r="C55" s="0" t="n">
@@ -1181,24 +1382,24 @@
       <c r="D55" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="E55" s="3" t="s">
+      <c r="E55" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="56" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="3" t="s">
+    <row r="56" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B56" s="3" t="s">
+      <c r="B56" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="C56" s="3" t="n">
+      <c r="C56" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="D56" s="3" t="s">
+      <c r="D56" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="E56" s="3" t="s">
+      <c r="E56" s="4" t="s">
         <v>47</v>
       </c>
     </row>
@@ -1233,54 +1434,54 @@
         <v>49</v>
       </c>
     </row>
-    <row r="59" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="3" t="s">
+    <row r="59" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B59" s="3" t="s">
+      <c r="B59" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="C59" s="3" t="n">
+      <c r="C59" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="D59" s="3" t="s">
+      <c r="D59" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="E59" s="3" t="s">
+      <c r="E59" s="4" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="60" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="3" t="s">
+    <row r="60" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B60" s="3" t="s">
+      <c r="B60" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C60" s="3" t="n">
+      <c r="C60" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="D60" s="3" t="s">
+      <c r="D60" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="E60" s="3" t="s">
+      <c r="E60" s="4" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="61" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="3" t="s">
+    <row r="61" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B61" s="3" t="s">
+      <c r="B61" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="C61" s="3" t="n">
+      <c r="C61" s="4" t="n">
         <v>22</v>
       </c>
-      <c r="D61" s="3" t="s">
+      <c r="D61" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="E61" s="3" t="s">
+      <c r="E61" s="4" t="s">
         <v>56</v>
       </c>
     </row>
@@ -1310,7 +1511,7 @@
       <c r="A65" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="B65" s="3" t="s">
+      <c r="B65" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C65" s="0" t="n">
@@ -1319,7 +1520,7 @@
       <c r="D65" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="E65" s="3" t="s">
+      <c r="E65" s="4" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1336,7 +1537,7 @@
       <c r="D66" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="E66" s="3" t="s">
+      <c r="E66" s="4" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1361,7 +1562,7 @@
       <c r="A68" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="B68" s="3" t="s">
+      <c r="B68" s="4" t="s">
         <v>22</v>
       </c>
       <c r="C68" s="0" t="n">
@@ -1370,24 +1571,24 @@
       <c r="D68" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="E68" s="3" t="s">
+      <c r="E68" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="69" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="3" t="s">
+    <row r="69" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B69" s="3" t="s">
+      <c r="B69" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="C69" s="3" t="n">
+      <c r="C69" s="4" t="n">
         <v>22</v>
       </c>
-      <c r="D69" s="3" t="s">
+      <c r="D69" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="E69" s="3" t="s">
+      <c r="E69" s="4" t="s">
         <v>77</v>
       </c>
     </row>
@@ -1416,6 +1617,26 @@
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="2" t="s">
         <v>79</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="2" t="s">
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -1427,4 +1648,220 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A2:C39"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="5" width="26.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="5" width="19.77"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="6" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="4" style="5" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="C2" s="7" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="C3" s="8" t="n">
+        <f aca="false">33.12+245.7+27.49</f>
+        <v>306.31</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="C4" s="7" t="n">
+        <v>60.72</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="C5" s="8" t="n">
+        <v>372.3</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="C6" s="7" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="C7" s="8" t="n">
+        <v>16.06</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="C8" s="8" t="n">
+        <f aca="false">36*1.2*3</f>
+        <v>129.6</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C9" s="8"/>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C10" s="7" t="n">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C11" s="7" t="n">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C12" s="7"/>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="C13" s="7" t="n">
+        <v>34.1</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C14" s="7"/>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="C15" s="8" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C16" s="8"/>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="C17" s="7" t="n">
+        <f aca="false">183.52+168.01</f>
+        <v>351.53</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C18" s="8"/>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="C19" s="7" t="n">
+        <v>379.79</v>
+      </c>
+    </row>
+    <row r="22" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="C22" s="10" t="n">
+        <f aca="false">SUM(C2:C19)</f>
+        <v>1987.41</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C31" s="11"/>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C34" s="11"/>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C35" s="11"/>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C36" s="11"/>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C37" s="11"/>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C39" s="12"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>